<commit_message>
Added missing data for SUTD in GES 2018
</commit_message>
<xml_diff>
--- a/workbench/descriptive-analytics.xlsx
+++ b/workbench/descriptive-analytics.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sam\Desktop\MTech EBAC Sem 1\Practice Module\F5-APM\workbench\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A44A0A11-34FD-41AD-A026-A603EC2ED95F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22104972-6F73-45D2-BE10-9AAA910A289B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="19392" windowHeight="10392" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1685,7 +1685,7 @@
   <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>

</xml_diff>

<commit_message>
Ben: Added Tableau workbook
</commit_message>
<xml_diff>
--- a/workbench/descriptive-analytics.xlsx
+++ b/workbench/descriptive-analytics.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sam\Desktop\MTech EBAC Sem 1\Practice Module\F5-APM\workbench\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22104972-6F73-45D2-BE10-9AAA910A289B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F586C3F1-8019-4AF9-B842-1202DB767B4A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="19392" windowHeight="10392" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1376,7 +1376,7 @@
       <sheetName val="processed"/>
     </sheetNames>
     <sheetDataSet>
-      <sheetData sheetId="0"/>
+      <sheetData sheetId="0" refreshError="1"/>
       <sheetData sheetId="1">
         <row r="1">
           <cell r="C1" t="str">
@@ -1685,7 +1685,7 @@
   <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>

</xml_diff>

<commit_message>
Updated correlation graphs figures for consistency
</commit_message>
<xml_diff>
--- a/workbench/descriptive-analytics.xlsx
+++ b/workbench/descriptive-analytics.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sam\Desktop\MTech EBAC Sem 1\Practice Module\F5-APM\workbench\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{571E5AE1-5E05-4F23-95C5-16DCF260CD1F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46DC7441-9954-49AB-94F3-4276E8DC6E27}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="19392" windowHeight="10392" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,8 @@
     <externalReference r:id="rId5"/>
   </externalReferences>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'correl-gdp-employment'!$A$1:$C$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'correl-employment-GES'!$A$1:$D$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'correl-gdp-employment'!$D$1:$D$1</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -43,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="6">
   <si>
     <t>Year</t>
   </si>
@@ -51,17 +52,26 @@
     <t>Correlation between Singapore GDP and Employment</t>
   </si>
   <si>
-    <t>The correlation between these 2 factors are very strong</t>
+    <t>Correlation between Singapore Overall Employment and Graduate Employment</t>
   </si>
   <si>
-    <t>Correlation between Singapore Overall Employment and Graduate Employment</t>
+    <t>There is a very strong positive correlation between GDP and Overall Employment</t>
+  </si>
+  <si>
+    <t>Overall Employment [Millions]</t>
+  </si>
+  <si>
+    <t>Employed Graduates (thousands)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+  </numFmts>
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -71,6 +81,13 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -101,10 +118,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -126,11 +144,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -180,14 +199,14 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-SG"/>
+              <a:rPr lang="en-SG" sz="1800" u="sng"/>
               <a:t>Singapore GDP Vs</a:t>
             </a:r>
             <a:r>
-              <a:rPr lang="en-SG" baseline="0"/>
-              <a:t> Employment</a:t>
+              <a:rPr lang="en-SG" sz="1800" u="sng" baseline="0"/>
+              <a:t> Overall Employment</a:t>
             </a:r>
-            <a:endParaRPr lang="en-SG"/>
+            <a:endParaRPr lang="en-SG" sz="1800" u="sng"/>
           </a:p>
         </c:rich>
       </c:tx>
@@ -195,8 +214,8 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.24838188976377953"/>
-          <c:y val="3.2407407407407406E-2"/>
+          <c:x val="0.10945822397200351"/>
+          <c:y val="3.6062474098632405E-2"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="0"/>
@@ -246,6 +265,7 @@
                   <c:v>GDP At Current Market Prices [In millions (SGD)]</c:v>
                 </c:pt>
               </c:strCache>
+              <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart"/>
             </c:strRef>
           </c:tx>
           <c:spPr>
@@ -300,6 +320,7 @@
                 <a:endParaRPr lang="en-US"/>
               </a:p>
             </c:txPr>
+            <c:dLblPos val="b"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="1"/>
             <c:showCatName val="0"/>
@@ -307,7 +328,7 @@
             <c:showPercent val="0"/>
             <c:showBubbleSize val="0"/>
             <c:showLeaderLines val="0"/>
-            <c:extLst>
+            <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
@@ -329,10 +350,10 @@
           </c:dLbls>
           <c:xVal>
             <c:numRef>
-              <c:f>'correl-gdp-employment'!$A$2:$A$7</c:f>
+              <c:f>'correl-gdp-employment'!$A$2:$A$8</c:f>
               <c:numCache>
                 <c:formatCode>0</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>2013</c:v>
                 </c:pt>
@@ -351,15 +372,19 @@
                 <c:pt idx="5">
                   <c:v>2018</c:v>
                 </c:pt>
+                <c:pt idx="6">
+                  <c:v>2019</c:v>
+                </c:pt>
               </c:numCache>
+              <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart"/>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'correl-gdp-employment'!$B$2:$B$7</c:f>
+              <c:f>'correl-gdp-employment'!$B$2:$B$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>384870.3</c:v>
                 </c:pt>
@@ -378,32 +403,36 @@
                 <c:pt idx="5">
                   <c:v>507123.9</c:v>
                 </c:pt>
+                <c:pt idx="6">
+                  <c:v>510737.8</c:v>
+                </c:pt>
               </c:numCache>
+              <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart"/>
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-CC68-4BCF-ADA1-49122EE7AE57}"/>
+              <c16:uniqueId val="{00000001-63FE-429F-878C-E1081131C228}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
         <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
+          <c:idx val="3"/>
+          <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>'correl-gdp-employment'!$C$1</c:f>
+              <c:f>'correl-gdp-employment'!$D$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Employed (thousands)</c:v>
+                  <c:v>Overall Employment [Millions]</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="19050" cap="rnd">
+            <a:ln w="25400" cap="rnd">
               <a:noFill/>
               <a:round/>
             </a:ln>
@@ -414,11 +443,11 @@
             <c:size val="5"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent2"/>
+                <a:schemeClr val="accent4"/>
               </a:solidFill>
               <a:ln w="9525">
                 <a:solidFill>
-                  <a:schemeClr val="accent2"/>
+                  <a:schemeClr val="accent4"/>
                 </a:solidFill>
               </a:ln>
               <a:effectLst/>
@@ -454,6 +483,7 @@
                 <a:endParaRPr lang="en-US"/>
               </a:p>
             </c:txPr>
+            <c:dLblPos val="t"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="1"/>
             <c:showCatName val="0"/>
@@ -483,10 +513,10 @@
           </c:dLbls>
           <c:xVal>
             <c:numRef>
-              <c:f>'correl-gdp-employment'!$A$2:$A$7</c:f>
+              <c:f>'correl-gdp-employment'!$A$2:$A$8</c:f>
               <c:numCache>
                 <c:formatCode>0</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>2013</c:v>
                 </c:pt>
@@ -504,33 +534,39 @@
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>2018</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2019</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'correl-gdp-employment'!$C$2:$C$7</c:f>
+              <c:f>'correl-gdp-employment'!$D$2:$D$8</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:formatCode>_(* #,##0.00_);_(* \(#,##0.00\);_(* "-"??_);_(@_)</c:formatCode>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>3352.9</c:v>
+                  <c:v>3.3529</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3440.2</c:v>
+                  <c:v>3.4401999999999999</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3516</c:v>
+                  <c:v>3.516</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3570</c:v>
+                  <c:v>3.57</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3550.1</c:v>
+                  <c:v>3.5501</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3575.3</c:v>
+                  <c:v>3.5753000000000004</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3.6316999999999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -538,7 +574,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-CC68-4BCF-ADA1-49122EE7AE57}"/>
+              <c16:uniqueId val="{00000004-63FE-429F-878C-E1081131C228}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -552,6 +588,190 @@
         </c:dLbls>
         <c:axId val="913462111"/>
         <c:axId val="913453791"/>
+        <c:extLst>
+          <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+            <c15:filteredScatterSeries>
+              <c15:ser>
+                <c:idx val="1"/>
+                <c:order val="1"/>
+                <c:tx>
+                  <c:strRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>'correl-gdp-employment'!$C$1</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="1"/>
+                      <c:pt idx="0">
+                        <c:v>Employed (thousands)</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c:tx>
+                <c:spPr>
+                  <a:ln w="19050" cap="rnd">
+                    <a:noFill/>
+                    <a:round/>
+                  </a:ln>
+                  <a:effectLst/>
+                </c:spPr>
+                <c:marker>
+                  <c:symbol val="circle"/>
+                  <c:size val="5"/>
+                  <c:spPr>
+                    <a:solidFill>
+                      <a:schemeClr val="accent2"/>
+                    </a:solidFill>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="accent2"/>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c:marker>
+                <c:dLbls>
+                  <c:spPr>
+                    <a:noFill/>
+                    <a:ln>
+                      <a:noFill/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                  <c:txPr>
+                    <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                      <a:spAutoFit/>
+                    </a:bodyPr>
+                    <a:lstStyle/>
+                    <a:p>
+                      <a:pPr>
+                        <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                          <a:solidFill>
+                            <a:schemeClr val="tx1">
+                              <a:lumMod val="75000"/>
+                              <a:lumOff val="25000"/>
+                            </a:schemeClr>
+                          </a:solidFill>
+                          <a:latin typeface="+mn-lt"/>
+                          <a:ea typeface="+mn-ea"/>
+                          <a:cs typeface="+mn-cs"/>
+                        </a:defRPr>
+                      </a:pPr>
+                      <a:endParaRPr lang="en-US"/>
+                    </a:p>
+                  </c:txPr>
+                  <c:showLegendKey val="0"/>
+                  <c:showVal val="1"/>
+                  <c:showCatName val="0"/>
+                  <c:showSerName val="0"/>
+                  <c:showPercent val="0"/>
+                  <c:showBubbleSize val="0"/>
+                  <c:showLeaderLines val="0"/>
+                  <c:extLst>
+                    <c:ext uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                      <c15:showLeaderLines val="1"/>
+                      <c15:leaderLines>
+                        <c:spPr>
+                          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                            <a:solidFill>
+                              <a:schemeClr val="tx1">
+                                <a:lumMod val="35000"/>
+                                <a:lumOff val="65000"/>
+                              </a:schemeClr>
+                            </a:solidFill>
+                            <a:round/>
+                          </a:ln>
+                          <a:effectLst/>
+                        </c:spPr>
+                      </c15:leaderLines>
+                    </c:ext>
+                  </c:extLst>
+                </c:dLbls>
+                <c:xVal>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>'correl-gdp-employment'!$A$2:$A$8</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>0</c:formatCode>
+                      <c:ptCount val="7"/>
+                      <c:pt idx="0">
+                        <c:v>2013</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>2014</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>2015</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>2016</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>2017</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>2018</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>2019</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:xVal>
+                <c:yVal>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>'correl-gdp-employment'!$C$2:$C$8</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="7"/>
+                      <c:pt idx="0">
+                        <c:v>3352.9</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>3440.2</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>3516</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>3570</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>3550.1</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>3575.3</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>3631.7</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:yVal>
+                <c:smooth val="0"/>
+                <c:extLst>
+                  <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                    <c16:uniqueId val="{00000002-63FE-429F-878C-E1081131C228}"/>
+                  </c:ext>
+                </c:extLst>
+              </c15:ser>
+            </c15:filteredScatterSeries>
+          </c:ext>
+        </c:extLst>
       </c:scatterChart>
       <c:valAx>
         <c:axId val="913462111"/>
@@ -619,7 +839,7 @@
       <c:valAx>
         <c:axId val="913453791"/>
         <c:scaling>
-          <c:logBase val="1000"/>
+          <c:logBase val="100"/>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="1"/>
@@ -639,7 +859,7 @@
           </c:spPr>
         </c:majorGridlines>
         <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
+        <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:crossAx val="913462111"/>
@@ -763,12 +983,12 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-SG"/>
-              <a:t>Overall VS</a:t>
+              <a:rPr lang="en-SG" sz="1600" b="1" u="sng"/>
+              <a:t>Singapore Overall VS</a:t>
             </a:r>
             <a:r>
-              <a:rPr lang="en-SG" baseline="0"/>
-              <a:t> Graduate Employment (Singapore)</a:t>
+              <a:rPr lang="en-SG" sz="1600" b="1" u="sng" baseline="0"/>
+              <a:t> Graduate Employment</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -811,7 +1031,7 @@
           <c:yMode val="edge"/>
           <c:x val="5.5888888888888891E-2"/>
           <c:y val="0.15160433272021254"/>
-          <c:w val="0.89149496937882766"/>
+          <c:w val="0.8591082785055455"/>
           <c:h val="0.61051188343946272"/>
         </c:manualLayout>
       </c:layout>
@@ -884,6 +1104,7 @@
                 <a:endParaRPr lang="en-US"/>
               </a:p>
             </c:txPr>
+            <c:dLblPos val="r"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="1"/>
             <c:showCatName val="0"/>
@@ -979,15 +1200,15 @@
           </c:extLst>
         </c:ser>
         <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
+          <c:idx val="2"/>
+          <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>'correl-employment-GES'!$C$1</c:f>
+              <c:f>'correl-employment-GES'!$D$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Employed Graduates</c:v>
+                  <c:v>Employed Graduates (thousands)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1004,11 +1225,11 @@
             <c:size val="5"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent2"/>
+                <a:srgbClr val="FFC000"/>
               </a:solidFill>
               <a:ln w="9525">
                 <a:solidFill>
-                  <a:schemeClr val="accent2"/>
+                  <a:schemeClr val="accent3"/>
                 </a:solidFill>
               </a:ln>
               <a:effectLst/>
@@ -1044,6 +1265,7 @@
                 <a:endParaRPr lang="en-US"/>
               </a:p>
             </c:txPr>
+            <c:dLblPos val="r"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="1"/>
             <c:showCatName val="0"/>
@@ -1103,30 +1325,30 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'correl-employment-GES'!$C$2:$C$8</c:f>
+              <c:f>'correl-employment-GES'!$D$2:$D$8</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>10029</c:v>
+                  <c:v>10.029</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>10167</c:v>
+                  <c:v>10.167</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>10337</c:v>
+                  <c:v>10.337</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>10944</c:v>
+                  <c:v>10.944000000000001</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>12551</c:v>
+                  <c:v>12.551</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>12626</c:v>
+                  <c:v>12.625999999999999</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>12900</c:v>
+                  <c:v>12.9</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1134,7 +1356,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-7AFB-40FB-8F55-D26DE7BD6F0F}"/>
+              <c16:uniqueId val="{00000001-ADC1-430E-B3B9-8BA57DC08FC1}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1148,11 +1370,197 @@
         </c:dLbls>
         <c:axId val="316179407"/>
         <c:axId val="316179823"/>
+        <c:extLst>
+          <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+            <c15:filteredScatterSeries>
+              <c15:ser>
+                <c:idx val="1"/>
+                <c:order val="1"/>
+                <c:tx>
+                  <c:strRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>'correl-employment-GES'!$C$1</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="1"/>
+                      <c:pt idx="0">
+                        <c:v>Employed Graduates</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c:tx>
+                <c:spPr>
+                  <a:ln w="25400" cap="rnd">
+                    <a:noFill/>
+                    <a:round/>
+                  </a:ln>
+                  <a:effectLst/>
+                </c:spPr>
+                <c:marker>
+                  <c:symbol val="circle"/>
+                  <c:size val="5"/>
+                  <c:spPr>
+                    <a:solidFill>
+                      <a:schemeClr val="accent2"/>
+                    </a:solidFill>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="accent2"/>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c:marker>
+                <c:dLbls>
+                  <c:spPr>
+                    <a:noFill/>
+                    <a:ln>
+                      <a:noFill/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                  <c:txPr>
+                    <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                      <a:spAutoFit/>
+                    </a:bodyPr>
+                    <a:lstStyle/>
+                    <a:p>
+                      <a:pPr>
+                        <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                          <a:solidFill>
+                            <a:schemeClr val="tx1">
+                              <a:lumMod val="75000"/>
+                              <a:lumOff val="25000"/>
+                            </a:schemeClr>
+                          </a:solidFill>
+                          <a:latin typeface="+mn-lt"/>
+                          <a:ea typeface="+mn-ea"/>
+                          <a:cs typeface="+mn-cs"/>
+                        </a:defRPr>
+                      </a:pPr>
+                      <a:endParaRPr lang="en-US"/>
+                    </a:p>
+                  </c:txPr>
+                  <c:showLegendKey val="0"/>
+                  <c:showVal val="1"/>
+                  <c:showCatName val="0"/>
+                  <c:showSerName val="0"/>
+                  <c:showPercent val="0"/>
+                  <c:showBubbleSize val="0"/>
+                  <c:showLeaderLines val="0"/>
+                  <c:extLst>
+                    <c:ext uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                      <c15:showLeaderLines val="1"/>
+                      <c15:leaderLines>
+                        <c:spPr>
+                          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                            <a:solidFill>
+                              <a:schemeClr val="tx1">
+                                <a:lumMod val="35000"/>
+                                <a:lumOff val="65000"/>
+                              </a:schemeClr>
+                            </a:solidFill>
+                            <a:round/>
+                          </a:ln>
+                          <a:effectLst/>
+                        </c:spPr>
+                      </c15:leaderLines>
+                    </c:ext>
+                  </c:extLst>
+                </c:dLbls>
+                <c:xVal>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>'correl-employment-GES'!$A$2:$A$8</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="7"/>
+                      <c:pt idx="0">
+                        <c:v>2013</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>2014</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>2015</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>2016</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>2017</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>2018</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>2019</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:xVal>
+                <c:yVal>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>'correl-employment-GES'!$C$2:$C$8</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="7"/>
+                      <c:pt idx="0">
+                        <c:v>10029</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>10167</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>10337</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>10944</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>12551</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>12626</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>12900</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:yVal>
+                <c:smooth val="0"/>
+                <c:extLst>
+                  <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                    <c16:uniqueId val="{00000001-7AFB-40FB-8F55-D26DE7BD6F0F}"/>
+                  </c:ext>
+                </c:extLst>
+              </c15:ser>
+            </c15:filteredScatterSeries>
+          </c:ext>
+        </c:extLst>
       </c:scatterChart>
       <c:valAx>
         <c:axId val="316179407"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="2019"/>
+          <c:min val="2013"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
@@ -1214,6 +1622,7 @@
       <c:valAx>
         <c:axId val="316179823"/>
         <c:scaling>
+          <c:logBase val="10"/>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="1"/>
@@ -1233,7 +1642,7 @@
           </c:spPr>
         </c:majorGridlines>
         <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
+        <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:crossAx val="316179407"/>
@@ -1249,17 +1658,7 @@
       </c:spPr>
     </c:plotArea>
     <c:legend>
-      <c:legendPos val="r"/>
-      <c:layout>
-        <c:manualLayout>
-          <c:xMode val="edge"/>
-          <c:yMode val="edge"/>
-          <c:x val="0.18938385826771653"/>
-          <c:y val="0.8262370637146752"/>
-          <c:w val="0.61894947506561682"/>
-          <c:h val="0.13795314212332901"/>
-        </c:manualLayout>
-      </c:layout>
+      <c:legendPos val="b"/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2449,16 +2848,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>390525</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>177165</xdr:rowOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>440055</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>219075</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>481965</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>177165</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>531495</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>36195</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2490,16 +2889,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>209550</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>245744</xdr:rowOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>320040</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>441960</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>300990</xdr:colOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>297180</xdr:colOff>
       <xdr:row>9</xdr:row>
-      <xdr:rowOff>609599</xdr:rowOff>
+      <xdr:rowOff>845819</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2972,10 +3371,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="N8" sqref="N8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -2983,9 +3382,10 @@
     <col min="1" max="1" width="19.578125" customWidth="1"/>
     <col min="2" max="2" width="21.83984375" customWidth="1"/>
     <col min="3" max="3" width="14.7890625" customWidth="1"/>
+    <col min="4" max="4" width="19.7890625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:4" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2997,8 +3397,11 @@
         <f>[2]processed!$C1</f>
         <v>Employed (thousands)</v>
       </c>
+      <c r="D1" s="3" t="s">
+        <v>4</v>
+      </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="4">
         <v>2013</v>
       </c>
@@ -3010,8 +3413,12 @@
         <f>[2]processed!$C2</f>
         <v>3352.9</v>
       </c>
+      <c r="D2" s="10">
+        <f>C2/1000</f>
+        <v>3.3529</v>
+      </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="4">
         <v>2014</v>
       </c>
@@ -3023,8 +3430,12 @@
         <f>[2]processed!$C3</f>
         <v>3440.2</v>
       </c>
+      <c r="D3" s="10">
+        <f t="shared" ref="D3:D8" si="0">C3/1000</f>
+        <v>3.4401999999999999</v>
+      </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="4">
         <v>2015</v>
       </c>
@@ -3036,8 +3447,12 @@
         <f>[2]processed!$C4</f>
         <v>3516</v>
       </c>
+      <c r="D4" s="10">
+        <f t="shared" si="0"/>
+        <v>3.516</v>
+      </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="4">
         <v>2016</v>
       </c>
@@ -3049,8 +3464,12 @@
         <f>[2]processed!$C5</f>
         <v>3570</v>
       </c>
+      <c r="D5" s="10">
+        <f t="shared" si="0"/>
+        <v>3.57</v>
+      </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="4">
         <v>2017</v>
       </c>
@@ -3062,8 +3481,12 @@
         <f>[2]processed!$C6</f>
         <v>3550.1</v>
       </c>
+      <c r="D6" s="10">
+        <f t="shared" si="0"/>
+        <v>3.5501</v>
+      </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="4">
         <v>2018</v>
       </c>
@@ -3075,8 +3498,12 @@
         <f>[2]processed!$C7</f>
         <v>3575.3</v>
       </c>
+      <c r="D7" s="10">
+        <f t="shared" si="0"/>
+        <v>3.5753000000000004</v>
+      </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="4">
         <v>2019</v>
       </c>
@@ -3088,32 +3515,38 @@
         <f>[2]processed!$C8</f>
         <v>3631.7</v>
       </c>
+      <c r="D8" s="10">
+        <f t="shared" si="0"/>
+        <v>3.6316999999999999</v>
+      </c>
     </row>
-    <row r="10" spans="1:3" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:4" ht="86.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="5" t="s">
         <v>1</v>
       </c>
       <c r="B10" s="6">
-        <f>CORREL(B2:B8,C2:C8)</f>
-        <v>0.88844523945303933</v>
+        <f>CORREL(B2:B8,D2:D8)</f>
+        <v>0.88844523945303988</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>2</v>
-      </c>
+        <v>3</v>
+      </c>
+      <c r="D10" s="9"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:C1" xr:uid="{5819F6C0-DE79-4CB3-BFF1-E843E31FC0F5}"/>
+  <autoFilter ref="D1" xr:uid="{FD0C94DF-6853-44CD-94D7-8E9221A60A65}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{134DC496-8FC5-4225-BA33-085BD38A64CD}">
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:D10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="O3" sqref="O3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -3121,22 +3554,26 @@
     <col min="1" max="1" width="16.15625" customWidth="1"/>
     <col min="2" max="2" width="15" customWidth="1"/>
     <col min="3" max="3" width="15.5234375" customWidth="1"/>
+    <col min="4" max="4" width="10.41796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" t="s">
+    <row r="1" spans="1:4" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="8" t="str">
+      <c r="B1" s="3" t="str">
         <f>[2]processed!$C1</f>
         <v>Employed (thousands)</v>
       </c>
-      <c r="C1" s="8" t="str">
+      <c r="C1" s="3" t="str">
         <f>'[3]overall-grad-employment'!$D1</f>
         <v>Employed Graduates</v>
       </c>
+      <c r="D1" s="3" t="s">
+        <v>5</v>
+      </c>
     </row>
-    <row r="2" spans="1:3" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:4" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A2">
         <v>2013</v>
       </c>
@@ -3148,8 +3585,12 @@
         <f>'[3]overall-grad-employment'!$D2</f>
         <v>10029</v>
       </c>
+      <c r="D2" s="11">
+        <f>C2/1000</f>
+        <v>10.029</v>
+      </c>
     </row>
-    <row r="3" spans="1:3" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A3">
         <v>2014</v>
       </c>
@@ -3161,8 +3602,12 @@
         <f>'[3]overall-grad-employment'!$D3</f>
         <v>10167</v>
       </c>
+      <c r="D3" s="11">
+        <f t="shared" ref="D3:D8" si="0">C3/1000</f>
+        <v>10.167</v>
+      </c>
     </row>
-    <row r="4" spans="1:3" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A4">
         <v>2015</v>
       </c>
@@ -3174,8 +3619,12 @@
         <f>'[3]overall-grad-employment'!$D4</f>
         <v>10337</v>
       </c>
+      <c r="D4" s="11">
+        <f t="shared" si="0"/>
+        <v>10.337</v>
+      </c>
     </row>
-    <row r="5" spans="1:3" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A5">
         <v>2016</v>
       </c>
@@ -3187,8 +3636,12 @@
         <f>'[3]overall-grad-employment'!$D5</f>
         <v>10944</v>
       </c>
+      <c r="D5" s="11">
+        <f t="shared" si="0"/>
+        <v>10.944000000000001</v>
+      </c>
     </row>
-    <row r="6" spans="1:3" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A6">
         <v>2017</v>
       </c>
@@ -3200,8 +3653,12 @@
         <f>'[3]overall-grad-employment'!$D6</f>
         <v>12551</v>
       </c>
+      <c r="D6" s="11">
+        <f t="shared" si="0"/>
+        <v>12.551</v>
+      </c>
     </row>
-    <row r="7" spans="1:3" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A7">
         <v>2018</v>
       </c>
@@ -3213,8 +3670,12 @@
         <f>'[3]overall-grad-employment'!$D7</f>
         <v>12626</v>
       </c>
+      <c r="D7" s="11">
+        <f t="shared" si="0"/>
+        <v>12.625999999999999</v>
+      </c>
     </row>
-    <row r="8" spans="1:3" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A8">
         <v>2019</v>
       </c>
@@ -3226,20 +3687,25 @@
         <f>'[3]overall-grad-employment'!$D8</f>
         <v>12900</v>
       </c>
+      <c r="D8" s="11">
+        <f t="shared" si="0"/>
+        <v>12.9</v>
+      </c>
     </row>
-    <row r="10" spans="1:3" ht="86.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:4" ht="86.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="8" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B10" s="6">
         <f>CORREL(B2:B8,C2:C8)</f>
         <v>0.80097164711304802</v>
       </c>
-      <c r="C10" s="9" t="s">
-        <v>2</v>
+      <c r="C10" s="7" t="s">
+        <v>3</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:D1" xr:uid="{E08878BB-A919-45B1-855D-C4B7CDADACE1}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Updated Correlation Charts for Singapore GDP vs Employment and Employment vs Grad Employment in tableau
</commit_message>
<xml_diff>
--- a/workbench/descriptive-analytics.xlsx
+++ b/workbench/descriptive-analytics.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sam\Desktop\MTech EBAC Sem 1\Practice Module\F5-APM\workbench\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46DC7441-9954-49AB-94F3-4276E8DC6E27}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2F58739-1C68-4DF0-8A6C-77693D46C511}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="19392" windowHeight="10392" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3545,8 +3545,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{134DC496-8FC5-4225-BA33-085BD38A64CD}">
   <dimension ref="A1:D10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="O3" sqref="O3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>

</xml_diff>